<commit_message>
msz - some first steps with mobile and desktop
</commit_message>
<xml_diff>
--- a/Data/Dialogs/dlgLogin.xlsx
+++ b/Data/Dialogs/dlgLogin.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\OnTop\Data\Dialogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA3F5EAF-E9EB-4A49-8450-163050C2D454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1132A9CF-389F-46DE-8ED6-4024A0932D49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2736" yWindow="708" windowWidth="35220" windowHeight="15300" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
+    <workbookView xWindow="2496" yWindow="1980" windowWidth="38784" windowHeight="15300" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -236,7 +236,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1598995</xdr:colOff>
+      <xdr:colOff>966535</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>109873</xdr:rowOff>
     </xdr:to>
@@ -574,18 +574,18 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="42.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.21875" customWidth="1"/>
-    <col min="3" max="3" width="14.21875" customWidth="1"/>
+    <col min="3" max="3" width="23.44140625" customWidth="1"/>
     <col min="4" max="4" width="48.33203125" customWidth="1"/>
     <col min="5" max="5" width="75.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.109375" customWidth="1"/>
-    <col min="7" max="7" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="42.88671875" customWidth="1"/>
     <col min="8" max="8" width="21.6640625" customWidth="1"/>
     <col min="9" max="9" width="19.44140625" customWidth="1"/>
     <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
msz - erste Experimente mit AppiumLibrary
</commit_message>
<xml_diff>
--- a/Data/Dialogs/dlgLogin.xlsx
+++ b/Data/Dialogs/dlgLogin.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\OnTop\Data\Dialogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1132A9CF-389F-46DE-8ED6-4024A0932D49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B1E310C-B2D1-4D39-9CCE-6CEBB1BA0EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2496" yWindow="1980" windowWidth="38784" windowHeight="15300" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
+    <workbookView xWindow="2124" yWindow="864" windowWidth="23004" windowHeight="15300" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="51">
   <si>
     <t>txtEmailAdresse</t>
   </si>
@@ -160,6 +160,24 @@
   </si>
   <si>
     <t>&lt;GETPASSWORD&gt;</t>
+  </si>
+  <si>
+    <t>Login mit Gast-Rolle</t>
+  </si>
+  <si>
+    <t>info@matthias-schmotz.de</t>
+  </si>
+  <si>
+    <t>Login mit Mitglied-Rolle</t>
+  </si>
+  <si>
+    <t>Login mit Trainer-Rolle</t>
+  </si>
+  <si>
+    <t>matthias@matthias-schmotz.eu</t>
+  </si>
+  <si>
+    <t>funtestic@matthias-schmotz.de</t>
   </si>
 </sst>
 </file>
@@ -204,9 +222,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -230,15 +250,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>966535</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>109873</xdr:rowOff>
+      <xdr:colOff>951295</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>140353</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -261,7 +281,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15240" y="2308860"/>
+          <a:off x="0" y="3253740"/>
           <a:ext cx="9638095" cy="4933333"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -571,255 +591,314 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82737E07-8287-4E6B-9130-6C87B574EFB8}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.21875" customWidth="1"/>
-    <col min="3" max="3" width="23.44140625" customWidth="1"/>
-    <col min="4" max="4" width="48.33203125" customWidth="1"/>
-    <col min="5" max="5" width="75.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.109375" customWidth="1"/>
-    <col min="7" max="7" width="42.88671875" customWidth="1"/>
-    <col min="8" max="8" width="21.6640625" customWidth="1"/>
-    <col min="9" max="9" width="19.44140625" customWidth="1"/>
-    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13" customWidth="1"/>
+    <col min="1" max="1" width="42.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="48.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="75.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="42.88671875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="19.44140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="1"/>
-      <c r="G10" t="s">
+      <c r="F10" s="2"/>
+      <c r="G10" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L11" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L12" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L15" s="1" t="s">
         <v>23</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="G10" r:id="rId1" xr:uid="{330831B1-92CC-461F-896F-5B43547B3CB3}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
msz - Starting second Login-Testcase + var-handling
</commit_message>
<xml_diff>
--- a/Data/Dialogs/dlgLogin.xlsx
+++ b/Data/Dialogs/dlgLogin.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\OnTop\Data\Dialogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE03058-F5D1-4FFB-8B72-E9F1591F23BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AECCA191-4C6A-4879-B79A-CF3EEAE51428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3216" yWindow="888" windowWidth="37188" windowHeight="15300" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
+    <workbookView xWindow="8052" yWindow="288" windowWidth="26088" windowHeight="15300" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="64">
   <si>
     <t>txtEmailAdresse</t>
   </si>
@@ -214,6 +214,9 @@
   </si>
   <si>
     <t>xpath=//*[@hint='PASSWORT:']</t>
+  </si>
+  <si>
+    <t>Funktioniert noch nicht</t>
   </si>
 </sst>
 </file>
@@ -655,10 +658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82737E07-8287-4E6B-9130-6C87B574EFB8}">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -921,8 +924,11 @@
       <c r="B12" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="J12" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="L12" s="1" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -997,6 +1003,17 @@
       </c>
       <c r="L16" s="1" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>